<commit_message>
Updated schedule and altered run list to reflect notes taken from meeting with Markus: better to run reference genes for one sample group first to compare which genes should be run for group 2.
</commit_message>
<xml_diff>
--- a/September_Schedule.xlsx
+++ b/September_Schedule.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -49,19 +49,19 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">meet with Zsolt (?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run survival extracts, Meet with markus, qPCR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">meet with Zsolt (?), qPCR</t>
+    <t xml:space="preserve"> Meet with markus, qPCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meet with Zsolt, Survival control extraction, run queens and random bee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qPCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benji’s defense, derivatisation with Zsolt if time allows</t>
   </si>
   <si>
     <t xml:space="preserve">Run survival extracts, qPCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extractions and concentrations</t>
   </si>
   <si>
     <t xml:space="preserve">qPCR</t>
@@ -86,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,7 +146,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,7 +155,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,8 +163,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -186,12 +191,13 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,7 +230,7 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -252,100 +258,100 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" customFormat="false" ht="117.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>44802</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="4" t="n">
         <v>44809</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="4" t="n">
         <v>44816</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="4" t="n">
         <v>44823</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="4" t="n">
         <v>44830</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Finished script automisation, updated schedule and currently working on correcting chromatogram alignment.
</commit_message>
<xml_diff>
--- a/September_Schedule.xlsx
+++ b/September_Schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t xml:space="preserve">Week beginning</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve"> qPCR</t>
   </si>
   <si>
-    <t xml:space="preserve">Benji’s defense, derivatisation with Zsolt if time allows</t>
+    <t xml:space="preserve">Benji’s defense, derivatisation with Zsolt</t>
   </si>
   <si>
     <t xml:space="preserve">Run survival extracts, qPCR</t>
@@ -191,10 +191,10 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.81"/>
@@ -258,7 +258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="117.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>44802</v>
       </c>
@@ -293,20 +293,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>44809</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">

</xml_diff>

<commit_message>
Updated README files, completed master table for Flying/Not Flying experiment and sorted GCMS files/ repository
</commit_message>
<xml_diff>
--- a/September_Schedule.xlsx
+++ b/September_Schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t xml:space="preserve">Week beginning</t>
   </si>
@@ -210,10 +210,10 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.26"/>
@@ -383,35 +383,75 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>44823</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>44830</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>